<commit_message>
vault backup: 2025-03-14 13:15:31
</commit_message>
<xml_diff>
--- a/РАбОТА/Списание/Счета/Юго-Западный для списания.xlsx
+++ b/РАбОТА/Списание/Счета/Юго-Западный для списания.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esitnikov\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OBSIDIAN\DisparuDEP\РАбОТА\Списание\Счета\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1154AF91-401B-40AA-9032-3288FB3F89E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$G$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$B$1:$F$65</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="190">
   <si>
     <t>Дата</t>
   </si>
@@ -39,9 +38,6 @@
     <t>Информация</t>
   </si>
   <si>
-    <t>Организация</t>
-  </si>
-  <si>
     <t>Подразделение</t>
   </si>
   <si>
@@ -58,9 +54,6 @@
   </si>
   <si>
     <t xml:space="preserve">Юго-Западный Банк СБ РФ  </t>
-  </si>
-  <si>
-    <t>ООО "ДИИП-РЕГИОН"</t>
   </si>
   <si>
     <t>Регион</t>
@@ -609,7 +602,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -689,7 +682,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный_Лист1" xfId="1" xr:uid="{26053BF1-D7EF-4236-BAAE-FC0D2EE8343A}"/>
+    <cellStyle name="Обычный_Лист1" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -966,40 +959,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="69" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="69" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1007,1264 +1001,1099 @@
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E7" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E8" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E15" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E16" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E17" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E18" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E19" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E20" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E22" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>73</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E23" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>76</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E24" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>79</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E25" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>82</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E26" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>85</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E27" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>88</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E28" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E29" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>94</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E30" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E31" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>100</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E32" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>103</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>104</v>
+        <v>12</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>14</v>
+        <v>102</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>10</v>
+        <v>103</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>105</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E34" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>108</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>109</v>
+        <v>13</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>15</v>
+        <v>107</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>10</v>
+        <v>108</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>110</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E36" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>113</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E37" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>116</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E38" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>10</v>
+        <v>115</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>117</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E40" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>125</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E41" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>10</v>
+        <v>128</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>130</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E43" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>133</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>10</v>
+        <v>133</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>135</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E45" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>138</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>10</v>
+        <v>138</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>140</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E47" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>143</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>10</v>
+        <v>143</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>145</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E49" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>148</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E50" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>151</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>10</v>
+        <v>151</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>153</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E52" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>156</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>10</v>
+        <v>156</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B54" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E54" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>161</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>10</v>
+        <v>161</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>163</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>10</v>
+        <v>162</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>164</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -2272,210 +2101,183 @@
         <v>167</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>10</v>
+        <v>166</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>168</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E58" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>172</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>10</v>
+        <v>172</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>174</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E60" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E61" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>180</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>10</v>
+        <v>180</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>182</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E63" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>185</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E64" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>188</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E65" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>191</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G65" xr:uid="{A495A0C9-1E88-4AC8-A55B-3643E8447356}"/>
+  <autoFilter ref="A1:G65"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>